<commit_message>
worked on routine to process data fields
</commit_message>
<xml_diff>
--- a/sassie_variables_table.xlsx
+++ b/sassie_variables_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mzahn/github/SASSIE_downscale_ecco_v5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C3C100-48E9-8542-ACF8-9ACF46D595BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0190A8EC-738D-9946-86B2-A6B0D76C4B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="760" windowWidth="34540" windowHeight="20360" xr2:uid="{E4E239F0-85BC-1949-AD3A-4F3A4CE5C2C3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="106">
   <si>
     <t>n_dims</t>
   </si>
@@ -324,6 +324,36 @@
   </si>
   <si>
     <t>vec</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>cgrid_point</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>k_l</t>
+  </si>
+  <si>
+    <t>c w</t>
+  </si>
+  <si>
+    <t>mate</t>
   </si>
 </sst>
 </file>
@@ -359,8 +389,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,19 +706,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBAD622-170B-ED43-8388-3F6C8186C5D2}">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -709,11 +742,17 @@
       <c r="G1" t="s">
         <v>92</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -735,8 +774,14 @@
       <c r="G2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -758,8 +803,14 @@
       <c r="G3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -778,8 +829,14 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -798,8 +855,14 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -818,8 +881,17 @@
       <c r="F6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -839,7 +911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -859,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -879,7 +951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -902,7 +974,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -925,7 +997,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -945,7 +1017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -965,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -984,8 +1056,11 @@
       <c r="F14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1004,8 +1079,11 @@
       <c r="F15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1024,8 +1102,11 @@
       <c r="F16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1044,8 +1125,11 @@
       <c r="F17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1064,8 +1148,11 @@
       <c r="F18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1084,8 +1171,11 @@
       <c r="F19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1104,8 +1194,11 @@
       <c r="F20">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1124,8 +1217,11 @@
       <c r="F21">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1144,8 +1240,11 @@
       <c r="F22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1164,8 +1263,11 @@
       <c r="F23">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1184,8 +1286,11 @@
       <c r="F24">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1204,8 +1309,11 @@
       <c r="F25">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1224,8 +1332,11 @@
       <c r="F26">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1244,8 +1355,11 @@
       <c r="F27">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1264,8 +1378,11 @@
       <c r="F28">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1284,8 +1401,11 @@
       <c r="F29">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1304,8 +1424,11 @@
       <c r="F30">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1325,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1345,7 +1468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1365,7 +1488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1384,8 +1507,11 @@
       <c r="F34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1404,8 +1530,11 @@
       <c r="F35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1425,7 +1554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1445,7 +1574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1465,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1485,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1505,7 +1634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1525,7 +1654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1545,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1565,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1585,7 +1714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1605,7 +1734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1624,8 +1753,11 @@
       <c r="F46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1644,8 +1776,11 @@
       <c r="F47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1664,8 +1799,14 @@
       <c r="F48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" t="s">
+        <v>103</v>
+      </c>
+      <c r="I48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1684,8 +1825,14 @@
       <c r="F49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" t="s">
+        <v>103</v>
+      </c>
+      <c r="I49" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1704,8 +1851,11 @@
       <c r="F50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1724,8 +1874,11 @@
       <c r="F51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I51" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1744,8 +1897,11 @@
       <c r="F52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1764,8 +1920,11 @@
       <c r="F53">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1784,8 +1943,11 @@
       <c r="F54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I54" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1804,8 +1966,11 @@
       <c r="F55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1824,8 +1989,11 @@
       <c r="F56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I56" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1844,8 +2012,11 @@
       <c r="F57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1864,8 +2035,11 @@
       <c r="F58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I58" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1884,8 +2058,11 @@
       <c r="F59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I59" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1904,8 +2081,11 @@
       <c r="F60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I60" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1924,8 +2104,11 @@
       <c r="F61">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I61" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1944,8 +2127,11 @@
       <c r="F62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I62" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1964,8 +2150,11 @@
       <c r="F63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I63" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1984,8 +2173,11 @@
       <c r="F64">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2004,8 +2196,11 @@
       <c r="F65">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I65" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2024,8 +2219,11 @@
       <c r="F66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I66" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2044,8 +2242,11 @@
       <c r="F67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I67" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2063,6 +2264,9 @@
       </c>
       <c r="F68">
         <v>2</v>
+      </c>
+      <c r="I68" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
processed u and v fields
</commit_message>
<xml_diff>
--- a/sassie_variables_table.xlsx
+++ b/sassie_variables_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mzahn/github/SASSIE_downscale_ecco_v5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0190A8EC-738D-9946-86B2-A6B0D76C4B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8C1DE0-F7B8-B847-8137-DF701730C8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="34540" windowHeight="20360" xr2:uid="{E4E239F0-85BC-1949-AD3A-4F3A4CE5C2C3}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="32300" windowHeight="20360" xr2:uid="{E4E239F0-85BC-1949-AD3A-4F3A4CE5C2C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="104">
   <si>
     <t>n_dims</t>
   </si>
@@ -323,15 +323,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>vec</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
     <t>cgrid_point</t>
   </si>
   <si>
@@ -347,21 +338,32 @@
     <t>top</t>
   </si>
   <si>
-    <t>k_l</t>
-  </si>
-  <si>
-    <t>c w</t>
-  </si>
-  <si>
     <t>mate</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>data_type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -389,14 +391,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -709,47 +741,52 @@
   <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="3"/>
     <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J1" t="s">
-        <v>105</v>
+      <c r="J1" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -772,13 +809,16 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="I2" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="J2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -801,13 +841,16 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="J3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -829,11 +872,17 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="G4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" t="s">
         <v>97</v>
       </c>
-      <c r="I4" t="s">
-        <v>100</v>
+      <c r="J4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -855,11 +904,17 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>97</v>
+      <c r="G5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="I5" t="s">
-        <v>101</v>
+        <v>98</v>
+      </c>
+      <c r="J5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -881,14 +936,17 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" t="s">
-        <v>102</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>97</v>
+      <c r="G6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="I6" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="J6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -910,6 +968,18 @@
       <c r="F7">
         <v>0</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -930,6 +1000,18 @@
       <c r="F8">
         <v>1</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J8" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -950,6 +1032,18 @@
       <c r="F9">
         <v>2</v>
       </c>
+      <c r="G9" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" t="s">
+        <v>96</v>
+      </c>
+      <c r="J9" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -971,6 +1065,15 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" t="s">
         <v>94</v>
       </c>
     </row>
@@ -994,6 +1097,15 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1015,6 +1127,18 @@
       </c>
       <c r="F12">
         <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J12" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1036,6 +1160,18 @@
       <c r="F13">
         <v>0</v>
       </c>
+      <c r="G13" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J13" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1056,8 +1192,17 @@
       <c r="F14">
         <v>0</v>
       </c>
+      <c r="G14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I14" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="J14" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1079,8 +1224,17 @@
       <c r="F15">
         <v>1</v>
       </c>
+      <c r="G15" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I15" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="J15" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1102,11 +1256,20 @@
       <c r="F16">
         <v>2</v>
       </c>
+      <c r="G16" t="s">
+        <v>101</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1125,11 +1288,20 @@
       <c r="F17">
         <v>3</v>
       </c>
+      <c r="G17" t="s">
+        <v>101</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1148,11 +1320,20 @@
       <c r="F18">
         <v>4</v>
       </c>
+      <c r="G18" t="s">
+        <v>101</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I18" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1171,11 +1352,20 @@
       <c r="F19">
         <v>5</v>
       </c>
+      <c r="G19" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1194,11 +1384,20 @@
       <c r="F20">
         <v>6</v>
       </c>
+      <c r="G20" t="s">
+        <v>101</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1217,11 +1416,20 @@
       <c r="F21">
         <v>7</v>
       </c>
+      <c r="G21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I21" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1240,11 +1448,20 @@
       <c r="F22">
         <v>8</v>
       </c>
+      <c r="G22" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I22" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1263,11 +1480,20 @@
       <c r="F23">
         <v>9</v>
       </c>
+      <c r="G23" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I23" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1286,11 +1512,20 @@
       <c r="F24">
         <v>10</v>
       </c>
+      <c r="G24" t="s">
+        <v>101</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1309,11 +1544,20 @@
       <c r="F25">
         <v>11</v>
       </c>
+      <c r="G25" t="s">
+        <v>101</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I25" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1332,11 +1576,20 @@
       <c r="F26">
         <v>12</v>
       </c>
+      <c r="G26" t="s">
+        <v>101</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I26" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1355,11 +1608,20 @@
       <c r="F27">
         <v>13</v>
       </c>
+      <c r="G27" t="s">
+        <v>101</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1378,11 +1640,20 @@
       <c r="F28">
         <v>14</v>
       </c>
+      <c r="G28" t="s">
+        <v>101</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I28" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1401,11 +1672,20 @@
       <c r="F29">
         <v>15</v>
       </c>
+      <c r="G29" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I29" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1424,11 +1704,20 @@
       <c r="F30">
         <v>16</v>
       </c>
+      <c r="G30" t="s">
+        <v>101</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1447,8 +1736,20 @@
       <c r="F31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>101</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I31" t="s">
+        <v>96</v>
+      </c>
+      <c r="J31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1467,8 +1768,20 @@
       <c r="F32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>101</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I32" t="s">
+        <v>96</v>
+      </c>
+      <c r="J32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1487,8 +1800,20 @@
       <c r="F33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I33" t="s">
+        <v>96</v>
+      </c>
+      <c r="J33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1507,11 +1832,20 @@
       <c r="F34">
         <v>3</v>
       </c>
+      <c r="G34" t="s">
+        <v>102</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I34" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="J34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1530,11 +1864,20 @@
       <c r="F35">
         <v>4</v>
       </c>
+      <c r="G35" t="s">
+        <v>102</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="J35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1553,8 +1896,20 @@
       <c r="F36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>101</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1573,8 +1928,20 @@
       <c r="F37">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>101</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1593,8 +1960,20 @@
       <c r="F38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>101</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1613,8 +1992,20 @@
       <c r="F39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>101</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1633,8 +2024,20 @@
       <c r="F40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>101</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1653,8 +2056,20 @@
       <c r="F41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>101</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1673,8 +2088,20 @@
       <c r="F42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>101</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1693,8 +2120,20 @@
       <c r="F43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>101</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1713,8 +2152,20 @@
       <c r="F44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G44" t="s">
+        <v>101</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1733,8 +2184,20 @@
       <c r="F45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G45" t="s">
+        <v>101</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1753,11 +2216,20 @@
       <c r="F46">
         <v>0</v>
       </c>
+      <c r="G46" t="s">
+        <v>102</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="J46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1776,11 +2248,20 @@
       <c r="F47">
         <v>1</v>
       </c>
+      <c r="G47" t="s">
+        <v>102</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I47" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="J47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1800,13 +2281,19 @@
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="I48" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1826,13 +2313,19 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="I49" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1851,11 +2344,20 @@
       <c r="F50">
         <v>0</v>
       </c>
+      <c r="G50" t="s">
+        <v>102</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I50" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="J50" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1874,11 +2376,20 @@
       <c r="F51">
         <v>1</v>
       </c>
+      <c r="G51" t="s">
+        <v>102</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I51" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="J51" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1897,11 +2408,20 @@
       <c r="F52">
         <v>2</v>
       </c>
+      <c r="G52" t="s">
+        <v>102</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I52" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="J52" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1920,11 +2440,20 @@
       <c r="F53">
         <v>3</v>
       </c>
+      <c r="G53" t="s">
+        <v>102</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I53" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="J53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1943,11 +2472,20 @@
       <c r="F54">
         <v>0</v>
       </c>
+      <c r="G54" t="s">
+        <v>102</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="I54" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="J54" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1966,11 +2504,20 @@
       <c r="F55">
         <v>1</v>
       </c>
+      <c r="G55" t="s">
+        <v>102</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="I55" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="J55" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1989,11 +2536,20 @@
       <c r="F56">
         <v>2</v>
       </c>
+      <c r="G56" t="s">
+        <v>102</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="I56" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="J56" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2012,11 +2568,20 @@
       <c r="F57">
         <v>3</v>
       </c>
+      <c r="G57" t="s">
+        <v>102</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="I57" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="J57" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2035,11 +2600,20 @@
       <c r="F58">
         <v>0</v>
       </c>
+      <c r="G58" t="s">
+        <v>101</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="I58" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J58" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2058,11 +2632,20 @@
       <c r="F59">
         <v>1</v>
       </c>
+      <c r="G59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="I59" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J59" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2081,11 +2664,20 @@
       <c r="F60">
         <v>2</v>
       </c>
+      <c r="G60" t="s">
+        <v>101</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="I60" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J60" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2104,11 +2696,20 @@
       <c r="F61">
         <v>3</v>
       </c>
+      <c r="G61" t="s">
+        <v>101</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="I61" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2127,11 +2728,20 @@
       <c r="F62">
         <v>0</v>
       </c>
+      <c r="G62" t="s">
+        <v>102</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="I62" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="J62" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2150,11 +2760,20 @@
       <c r="F63">
         <v>1</v>
       </c>
+      <c r="G63" t="s">
+        <v>102</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="I63" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="J63" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2173,11 +2792,20 @@
       <c r="F64">
         <v>2</v>
       </c>
+      <c r="G64" t="s">
+        <v>102</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="I64" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="J64" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2196,11 +2824,20 @@
       <c r="F65">
         <v>3</v>
       </c>
+      <c r="G65" t="s">
+        <v>102</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="I65" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="J65" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2219,11 +2856,20 @@
       <c r="F66">
         <v>0</v>
       </c>
+      <c r="G66" t="s">
+        <v>102</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="I66" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="J66" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2242,11 +2888,20 @@
       <c r="F67">
         <v>1</v>
       </c>
+      <c r="G67" t="s">
+        <v>102</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="I67" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="J67" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2265,11 +2920,25 @@
       <c r="F68">
         <v>2</v>
       </c>
+      <c r="G68" t="s">
+        <v>101</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="I68" t="s">
-        <v>104</v>
+        <v>96</v>
+      </c>
+      <c r="J68" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:J1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edits to table and plotting granules
</commit_message>
<xml_diff>
--- a/sassie_variables_table.xlsx
+++ b/sassie_variables_table.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mzahn/github/SASSIE_downscale_ecco_v5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3531E22-D7BB-AA4A-B357-3CD4787925D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E455855-C15E-8740-9870-24A98724C1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="760" windowWidth="34560" windowHeight="19900" xr2:uid="{E4E239F0-85BC-1949-AD3A-4F3A4CE5C2C3}"/>
+    <workbookView xWindow="-34260" yWindow="-7560" windowWidth="34260" windowHeight="28300" xr2:uid="{E4E239F0-85BC-1949-AD3A-4F3A4CE5C2C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$68</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="105">
   <si>
     <t>n_dims</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>data_type</t>
+  </si>
+  <si>
+    <t>variable_long_name</t>
   </si>
 </sst>
 </file>
@@ -719,25 +722,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBAD622-170B-ED43-8388-3F6C8186C5D2}">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -745,2176 +749,2179 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
-        <v>101</v>
-      </c>
       <c r="H2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" t="s">
         <v>93</v>
       </c>
-      <c r="I2" t="s">
-        <v>96</v>
-      </c>
       <c r="J2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>101</v>
-      </c>
       <c r="H3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" t="s">
         <v>93</v>
       </c>
-      <c r="I3" t="s">
-        <v>96</v>
-      </c>
       <c r="J3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>50</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>102</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>93</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>97</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>50</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>102</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>93</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>98</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>50</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6">
         <v>3</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>2</v>
       </c>
-      <c r="G6" t="s">
-        <v>101</v>
-      </c>
       <c r="H6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" t="s">
         <v>99</v>
       </c>
-      <c r="I6" t="s">
-        <v>96</v>
-      </c>
       <c r="J6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
         <v>3</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0</v>
       </c>
-      <c r="G7" t="s">
-        <v>101</v>
-      </c>
       <c r="H7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" t="s">
         <v>93</v>
       </c>
-      <c r="I7" t="s">
-        <v>96</v>
-      </c>
       <c r="J7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>35</v>
       </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
         <v>3</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
-        <v>101</v>
-      </c>
       <c r="H8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" t="s">
         <v>93</v>
       </c>
-      <c r="I8" t="s">
-        <v>96</v>
-      </c>
       <c r="J8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9">
         <v>3</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>2</v>
       </c>
-      <c r="G9" t="s">
-        <v>101</v>
-      </c>
       <c r="H9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I9" t="s">
         <v>93</v>
       </c>
-      <c r="I9" t="s">
-        <v>96</v>
-      </c>
       <c r="J9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>47</v>
       </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10">
         <v>3</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0</v>
       </c>
-      <c r="G10" t="s">
-        <v>101</v>
-      </c>
       <c r="H10" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>47</v>
       </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11">
         <v>3</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
-        <v>101</v>
-      </c>
       <c r="H11" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>49</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>47</v>
       </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12">
         <v>3</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>2</v>
       </c>
-      <c r="G12" t="s">
-        <v>101</v>
-      </c>
       <c r="H12" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>32</v>
       </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13">
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13">
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>0</v>
       </c>
-      <c r="G13" t="s">
-        <v>101</v>
-      </c>
       <c r="H13" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14">
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14">
         <v>17</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>0</v>
       </c>
-      <c r="G14" t="s">
-        <v>101</v>
-      </c>
       <c r="H14" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15">
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15">
         <v>17</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>1</v>
       </c>
-      <c r="G15" t="s">
-        <v>101</v>
-      </c>
       <c r="H15" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>30</v>
       </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16">
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16">
         <v>17</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>2</v>
       </c>
-      <c r="G16" t="s">
-        <v>101</v>
-      </c>
       <c r="H16" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>30</v>
       </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17">
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17">
         <v>17</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>3</v>
       </c>
-      <c r="G17" t="s">
-        <v>101</v>
-      </c>
       <c r="H17" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>30</v>
       </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18">
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18">
         <v>17</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>4</v>
       </c>
-      <c r="G18" t="s">
-        <v>101</v>
-      </c>
       <c r="H18" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>30</v>
       </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19">
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19">
         <v>17</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>5</v>
       </c>
-      <c r="G19" t="s">
-        <v>101</v>
-      </c>
       <c r="H19" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>30</v>
       </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20">
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20">
         <v>17</v>
       </c>
-      <c r="F20">
-        <v>6</v>
-      </c>
-      <c r="G20" t="s">
-        <v>101</v>
+      <c r="G20">
+        <v>6</v>
       </c>
       <c r="H20" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>30</v>
       </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21">
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21">
         <v>17</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>7</v>
       </c>
-      <c r="G21" t="s">
-        <v>101</v>
-      </c>
       <c r="H21" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>30</v>
       </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22">
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22">
         <v>17</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>8</v>
       </c>
-      <c r="G22" t="s">
-        <v>101</v>
-      </c>
       <c r="H22" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>30</v>
       </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23">
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
         <v>17</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>9</v>
       </c>
-      <c r="G23" t="s">
-        <v>101</v>
-      </c>
       <c r="H23" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>30</v>
       </c>
-      <c r="D24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24">
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24">
         <v>17</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>10</v>
       </c>
-      <c r="G24" t="s">
-        <v>101</v>
-      </c>
       <c r="H24" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J24" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>30</v>
       </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25">
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25">
         <v>17</v>
       </c>
-      <c r="F25">
-        <v>11</v>
-      </c>
-      <c r="G25" t="s">
-        <v>101</v>
+      <c r="G25">
+        <v>11</v>
       </c>
       <c r="H25" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>30</v>
       </c>
-      <c r="D26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26">
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26">
         <v>17</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>12</v>
       </c>
-      <c r="G26" t="s">
-        <v>101</v>
-      </c>
       <c r="H26" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J26" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>30</v>
       </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27">
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27">
         <v>17</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>13</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>102</v>
       </c>
-      <c r="H27" t="s">
-        <v>94</v>
-      </c>
       <c r="I27" t="s">
+        <v>94</v>
+      </c>
+      <c r="J27" t="s">
         <v>97</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>30</v>
       </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28">
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28">
         <v>17</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>14</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>102</v>
       </c>
-      <c r="H28" t="s">
-        <v>94</v>
-      </c>
       <c r="I28" t="s">
+        <v>94</v>
+      </c>
+      <c r="J28" t="s">
         <v>97</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>30</v>
       </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29">
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29">
         <v>17</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>15</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>102</v>
       </c>
-      <c r="H29" t="s">
-        <v>94</v>
-      </c>
       <c r="I29" t="s">
+        <v>94</v>
+      </c>
+      <c r="J29" t="s">
         <v>98</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>28</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>30</v>
       </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30">
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30">
         <v>17</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>16</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>102</v>
       </c>
-      <c r="H30" t="s">
-        <v>94</v>
-      </c>
       <c r="I30" t="s">
+        <v>94</v>
+      </c>
+      <c r="J30" t="s">
         <v>98</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>40</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>39</v>
       </c>
-      <c r="D31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31">
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31">
         <v>7</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>0</v>
       </c>
-      <c r="G31" t="s">
-        <v>101</v>
-      </c>
       <c r="H31" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J31" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>41</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>39</v>
       </c>
-      <c r="D32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32">
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32">
         <v>7</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>1</v>
       </c>
-      <c r="G32" t="s">
-        <v>101</v>
-      </c>
       <c r="H32" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J32" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>42</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>39</v>
       </c>
-      <c r="D33" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33">
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33">
         <v>7</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>2</v>
       </c>
-      <c r="G33" t="s">
-        <v>101</v>
-      </c>
       <c r="H33" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J33" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>43</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>39</v>
       </c>
-      <c r="D34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34">
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34">
         <v>7</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>3</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>102</v>
       </c>
-      <c r="H34" t="s">
-        <v>94</v>
-      </c>
       <c r="I34" t="s">
+        <v>94</v>
+      </c>
+      <c r="J34" t="s">
         <v>97</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>44</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>39</v>
       </c>
-      <c r="D35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35">
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35">
         <v>7</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>4</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>102</v>
       </c>
-      <c r="H35" t="s">
-        <v>94</v>
-      </c>
       <c r="I35" t="s">
+        <v>94</v>
+      </c>
+      <c r="J35" t="s">
         <v>98</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>45</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>39</v>
       </c>
-      <c r="D36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36">
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36">
         <v>7</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>5</v>
       </c>
-      <c r="G36" t="s">
-        <v>101</v>
-      </c>
       <c r="H36" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J36" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>46</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>39</v>
       </c>
-      <c r="D37" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37">
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37">
         <v>7</v>
       </c>
-      <c r="F37">
-        <v>6</v>
-      </c>
-      <c r="G37" t="s">
-        <v>101</v>
+      <c r="G37">
+        <v>6</v>
       </c>
       <c r="H37" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>51</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>54</v>
       </c>
-      <c r="D38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38">
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38">
         <v>3</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>0</v>
       </c>
-      <c r="G38" t="s">
-        <v>101</v>
-      </c>
       <c r="H38" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J38" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>52</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>54</v>
       </c>
-      <c r="D39" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39">
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39">
         <v>3</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>1</v>
       </c>
-      <c r="G39" t="s">
-        <v>101</v>
-      </c>
       <c r="H39" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J39" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>53</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>54</v>
       </c>
-      <c r="D40" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40">
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40">
         <v>3</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>2</v>
       </c>
-      <c r="G40" t="s">
-        <v>101</v>
-      </c>
       <c r="H40" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I40" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J40" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>56</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>55</v>
       </c>
-      <c r="D41" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41">
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41">
         <v>2</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>0</v>
       </c>
-      <c r="G41" t="s">
-        <v>101</v>
-      </c>
       <c r="H41" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I41" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J41" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>57</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>55</v>
       </c>
-      <c r="D42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42">
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42">
         <v>2</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>1</v>
       </c>
-      <c r="G42" t="s">
-        <v>101</v>
-      </c>
       <c r="H42" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J42" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>59</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>58</v>
       </c>
-      <c r="D43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43">
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43">
         <v>3</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>0</v>
       </c>
-      <c r="G43" t="s">
-        <v>101</v>
-      </c>
       <c r="H43" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J43" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>60</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>58</v>
       </c>
-      <c r="D44" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44">
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44">
         <v>3</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>1</v>
       </c>
-      <c r="G44" t="s">
-        <v>101</v>
-      </c>
       <c r="H44" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J44" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>61</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>58</v>
       </c>
-      <c r="D45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45">
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45">
         <v>3</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>2</v>
       </c>
-      <c r="G45" t="s">
-        <v>101</v>
-      </c>
       <c r="H45" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="I45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J45" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>63</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>62</v>
       </c>
-      <c r="D46" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46">
+      <c r="E46" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46">
         <v>2</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>0</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>102</v>
       </c>
-      <c r="H46" t="s">
-        <v>94</v>
-      </c>
       <c r="I46" t="s">
+        <v>94</v>
+      </c>
+      <c r="J46" t="s">
         <v>97</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>64</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>62</v>
       </c>
-      <c r="D47" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47">
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47">
         <v>2</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>1</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>102</v>
       </c>
-      <c r="H47" t="s">
-        <v>94</v>
-      </c>
       <c r="I47" t="s">
+        <v>94</v>
+      </c>
+      <c r="J47" t="s">
         <v>98</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>66</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>65</v>
       </c>
-      <c r="D48" t="s">
-        <v>6</v>
-      </c>
-      <c r="E48">
+      <c r="E48" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48">
         <v>2</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>0</v>
       </c>
-      <c r="G48" t="s">
-        <v>101</v>
-      </c>
       <c r="H48" t="s">
+        <v>101</v>
+      </c>
+      <c r="I48" t="s">
         <v>99</v>
       </c>
-      <c r="I48" t="s">
-        <v>96</v>
-      </c>
       <c r="J48" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>67</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>65</v>
       </c>
-      <c r="D49" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49">
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49">
         <v>2</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>1</v>
       </c>
-      <c r="G49" t="s">
-        <v>101</v>
-      </c>
       <c r="H49" t="s">
+        <v>101</v>
+      </c>
+      <c r="I49" t="s">
         <v>99</v>
       </c>
-      <c r="I49" t="s">
-        <v>96</v>
-      </c>
       <c r="J49" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>69</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>68</v>
       </c>
-      <c r="D50" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50">
+      <c r="E50" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50">
         <v>4</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>0</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>102</v>
       </c>
-      <c r="H50" t="s">
-        <v>94</v>
-      </c>
       <c r="I50" t="s">
+        <v>94</v>
+      </c>
+      <c r="J50" t="s">
         <v>97</v>
       </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>70</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>68</v>
       </c>
-      <c r="D51" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51">
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51">
         <v>4</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>1</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>102</v>
       </c>
-      <c r="H51" t="s">
-        <v>94</v>
-      </c>
       <c r="I51" t="s">
+        <v>94</v>
+      </c>
+      <c r="J51" t="s">
         <v>97</v>
       </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>71</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>68</v>
       </c>
-      <c r="D52" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52">
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52">
         <v>4</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>2</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>102</v>
       </c>
-      <c r="H52" t="s">
-        <v>94</v>
-      </c>
       <c r="I52" t="s">
+        <v>94</v>
+      </c>
+      <c r="J52" t="s">
         <v>98</v>
       </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>72</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>68</v>
       </c>
-      <c r="D53" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53">
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53">
         <v>4</v>
       </c>
-      <c r="F53">
+      <c r="G53">
         <v>3</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>102</v>
       </c>
-      <c r="H53" t="s">
-        <v>94</v>
-      </c>
       <c r="I53" t="s">
+        <v>94</v>
+      </c>
+      <c r="J53" t="s">
         <v>98</v>
       </c>
-      <c r="J53" t="s">
+      <c r="K53" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>74</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>73</v>
       </c>
-      <c r="D54" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54">
+      <c r="E54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54">
         <v>4</v>
       </c>
-      <c r="F54">
+      <c r="G54">
         <v>0</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>102</v>
       </c>
-      <c r="H54" t="s">
+      <c r="I54" t="s">
         <v>93</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>97</v>
       </c>
-      <c r="J54" t="s">
+      <c r="K54" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>75</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>73</v>
       </c>
-      <c r="D55" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55">
+      <c r="E55" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55">
         <v>4</v>
       </c>
-      <c r="F55">
+      <c r="G55">
         <v>1</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>102</v>
       </c>
-      <c r="H55" t="s">
+      <c r="I55" t="s">
         <v>93</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>97</v>
       </c>
-      <c r="J55" t="s">
+      <c r="K55" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>76</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>73</v>
       </c>
-      <c r="D56" t="s">
-        <v>6</v>
-      </c>
-      <c r="E56">
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56">
         <v>4</v>
       </c>
-      <c r="F56">
+      <c r="G56">
         <v>2</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>102</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>93</v>
       </c>
-      <c r="I56" t="s">
+      <c r="J56" t="s">
         <v>98</v>
       </c>
-      <c r="J56" t="s">
+      <c r="K56" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>77</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>73</v>
       </c>
-      <c r="D57" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57">
+      <c r="E57" t="s">
+        <v>6</v>
+      </c>
+      <c r="F57">
         <v>4</v>
       </c>
-      <c r="F57">
+      <c r="G57">
         <v>3</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>102</v>
       </c>
-      <c r="H57" t="s">
+      <c r="I57" t="s">
         <v>93</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
         <v>98</v>
       </c>
-      <c r="J57" t="s">
+      <c r="K57" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>79</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>78</v>
       </c>
-      <c r="D58" t="s">
-        <v>6</v>
-      </c>
-      <c r="E58">
+      <c r="E58" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58">
         <v>4</v>
       </c>
-      <c r="F58">
+      <c r="G58">
         <v>0</v>
       </c>
-      <c r="G58" t="s">
-        <v>101</v>
-      </c>
       <c r="H58" t="s">
+        <v>101</v>
+      </c>
+      <c r="I58" t="s">
         <v>99</v>
       </c>
-      <c r="I58" t="s">
-        <v>96</v>
-      </c>
       <c r="J58" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K58" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>80</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>78</v>
       </c>
-      <c r="D59" t="s">
-        <v>6</v>
-      </c>
-      <c r="E59">
+      <c r="E59" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59">
         <v>4</v>
       </c>
-      <c r="F59">
+      <c r="G59">
         <v>1</v>
       </c>
-      <c r="G59" t="s">
-        <v>101</v>
-      </c>
       <c r="H59" t="s">
+        <v>101</v>
+      </c>
+      <c r="I59" t="s">
         <v>99</v>
       </c>
-      <c r="I59" t="s">
-        <v>96</v>
-      </c>
       <c r="J59" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K59" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>81</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>78</v>
       </c>
-      <c r="D60" t="s">
-        <v>6</v>
-      </c>
-      <c r="E60">
+      <c r="E60" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60">
         <v>4</v>
       </c>
-      <c r="F60">
+      <c r="G60">
         <v>2</v>
       </c>
-      <c r="G60" t="s">
-        <v>101</v>
-      </c>
       <c r="H60" t="s">
+        <v>101</v>
+      </c>
+      <c r="I60" t="s">
         <v>99</v>
       </c>
-      <c r="I60" t="s">
-        <v>96</v>
-      </c>
       <c r="J60" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K60" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>82</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>78</v>
       </c>
-      <c r="D61" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61">
+      <c r="E61" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61">
         <v>4</v>
       </c>
-      <c r="F61">
+      <c r="G61">
         <v>3</v>
       </c>
-      <c r="G61" t="s">
-        <v>101</v>
-      </c>
       <c r="H61" t="s">
+        <v>101</v>
+      </c>
+      <c r="I61" t="s">
         <v>99</v>
       </c>
-      <c r="I61" t="s">
-        <v>96</v>
-      </c>
       <c r="J61" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="K61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>84</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>83</v>
       </c>
-      <c r="D62" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62">
+      <c r="E62" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62">
         <v>4</v>
       </c>
-      <c r="F62">
+      <c r="G62">
         <v>0</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>102</v>
       </c>
-      <c r="H62" t="s">
+      <c r="I62" t="s">
         <v>93</v>
       </c>
-      <c r="I62" t="s">
+      <c r="J62" t="s">
         <v>97</v>
       </c>
-      <c r="J62" t="s">
+      <c r="K62" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>85</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>83</v>
       </c>
-      <c r="D63" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63">
+      <c r="E63" t="s">
+        <v>6</v>
+      </c>
+      <c r="F63">
         <v>4</v>
       </c>
-      <c r="F63">
+      <c r="G63">
         <v>1</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>102</v>
       </c>
-      <c r="H63" t="s">
+      <c r="I63" t="s">
         <v>93</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>97</v>
       </c>
-      <c r="J63" t="s">
+      <c r="K63" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>86</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>83</v>
       </c>
-      <c r="D64" t="s">
-        <v>6</v>
-      </c>
-      <c r="E64">
+      <c r="E64" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64">
         <v>4</v>
       </c>
-      <c r="F64">
+      <c r="G64">
         <v>2</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>102</v>
       </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>93</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>98</v>
       </c>
-      <c r="J64" t="s">
+      <c r="K64" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>87</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>83</v>
       </c>
-      <c r="D65" t="s">
-        <v>6</v>
-      </c>
-      <c r="E65">
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65">
         <v>4</v>
       </c>
-      <c r="F65">
+      <c r="G65">
         <v>3</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>102</v>
       </c>
-      <c r="H65" t="s">
+      <c r="I65" t="s">
         <v>93</v>
       </c>
-      <c r="I65" t="s">
+      <c r="J65" t="s">
         <v>98</v>
       </c>
-      <c r="J65" t="s">
+      <c r="K65" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>89</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>88</v>
       </c>
-      <c r="D66" t="s">
-        <v>6</v>
-      </c>
-      <c r="E66">
+      <c r="E66" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66">
         <v>3</v>
       </c>
-      <c r="F66">
+      <c r="G66">
         <v>0</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>102</v>
       </c>
-      <c r="H66" t="s">
+      <c r="I66" t="s">
         <v>93</v>
       </c>
-      <c r="I66" t="s">
+      <c r="J66" t="s">
         <v>97</v>
       </c>
-      <c r="J66" t="s">
+      <c r="K66" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>90</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>88</v>
       </c>
-      <c r="D67" t="s">
-        <v>6</v>
-      </c>
-      <c r="E67">
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67">
         <v>3</v>
       </c>
-      <c r="F67">
+      <c r="G67">
         <v>1</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>102</v>
       </c>
-      <c r="H67" t="s">
+      <c r="I67" t="s">
         <v>93</v>
       </c>
-      <c r="I67" t="s">
+      <c r="J67" t="s">
         <v>98</v>
       </c>
-      <c r="J67" t="s">
+      <c r="K67" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>91</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>88</v>
       </c>
-      <c r="D68" t="s">
-        <v>6</v>
-      </c>
-      <c r="E68">
+      <c r="E68" t="s">
+        <v>6</v>
+      </c>
+      <c r="F68">
         <v>3</v>
       </c>
-      <c r="F68">
+      <c r="G68">
         <v>2</v>
       </c>
-      <c r="G68" t="s">
-        <v>101</v>
-      </c>
       <c r="H68" t="s">
+        <v>101</v>
+      </c>
+      <c r="I68" t="s">
         <v>99</v>
       </c>
-      <c r="I68" t="s">
-        <v>96</v>
-      </c>
       <c r="J68" t="s">
+        <v>96</v>
+      </c>
+      <c r="K68" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:J1048576">
+  <conditionalFormatting sqref="A1:K1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>

</xml_diff>